<commit_message>
Include four quarters in data
</commit_message>
<xml_diff>
--- a/tests/artefacts/testdata.xlsx
+++ b/tests/artefacts/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/odi/liberia/aims/tests/artefacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069D8CD8-205B-8647-81EE-AC6B3DDF1B7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5B6905-B830-8745-BA6F-2C8CEB359C62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="980" windowWidth="27640" windowHeight="16020" xr2:uid="{0D2C3C09-8642-F64A-A841-4B349051A884}"/>
+    <workbookView xWindow="780" yWindow="820" windowWidth="27640" windowHeight="16020" xr2:uid="{0D2C3C09-8642-F64A-A841-4B349051A884}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>INFRASTRACTURE AND BASIC SERVICES</t>
+  </si>
+  <si>
+    <t>2018 Q3 (D)</t>
+  </si>
+  <si>
+    <t>2018 Q2 (D)</t>
+  </si>
+  <si>
+    <t>2018 Q1 (D)</t>
   </si>
 </sst>
 </file>
@@ -583,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75600FF7-6925-5A4F-B4D6-2E51A7284D2B}">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,9 +610,10 @@
     <col min="12" max="13" width="21.1640625" customWidth="1"/>
     <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,20 +668,29 @@
       <c r="R1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -720,24 +739,33 @@
       <c r="R2" s="2">
         <v>100</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0</v>
+      </c>
+      <c r="V2">
         <f ca="1">RANDBETWEEN(100,999)</f>
-        <v>163</v>
-      </c>
-      <c r="T2">
-        <f t="shared" ref="T2:V2" ca="1" si="0">RANDBETWEEN(100,999)</f>
-        <v>951</v>
-      </c>
-      <c r="U2">
+        <v>956</v>
+      </c>
+      <c r="W2">
+        <f t="shared" ref="W2:Y2" ca="1" si="0">RANDBETWEEN(100,999)</f>
+        <v>930</v>
+      </c>
+      <c r="X2">
         <f t="shared" ca="1" si="0"/>
-        <v>472</v>
-      </c>
-      <c r="V2">
+        <v>702</v>
+      </c>
+      <c r="Y2">
         <f t="shared" ca="1" si="0"/>
-        <v>148</v>
+        <v>957</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -786,24 +814,33 @@
       <c r="R3" s="2">
         <v>2000</v>
       </c>
-      <c r="S3">
-        <f t="shared" ref="S3:V11" ca="1" si="1">RANDBETWEEN(100,999)</f>
-        <v>182</v>
-      </c>
-      <c r="T3">
-        <f t="shared" ca="1" si="1"/>
-        <v>156</v>
-      </c>
-      <c r="U3">
-        <f t="shared" ca="1" si="1"/>
-        <v>190</v>
+      <c r="S3" s="2">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0</v>
       </c>
       <c r="V3">
-        <f t="shared" ca="1" si="1"/>
-        <v>770</v>
+        <f t="shared" ref="V3:Y11" ca="1" si="1">RANDBETWEEN(100,999)</f>
+        <v>776</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ca="1" si="1"/>
+        <v>157</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ca="1" si="1"/>
+        <v>758</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ca="1" si="1"/>
+        <v>924</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -855,24 +892,33 @@
       <c r="R4" s="2">
         <v>300</v>
       </c>
-      <c r="S4">
-        <f t="shared" ca="1" si="1"/>
-        <v>768</v>
-      </c>
-      <c r="T4">
-        <f t="shared" ca="1" si="1"/>
-        <v>326</v>
-      </c>
-      <c r="U4">
-        <f t="shared" ca="1" si="1"/>
-        <v>847</v>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="1"/>
-        <v>622</v>
+        <v>903</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ca="1" si="1"/>
+        <v>265</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ca="1" si="1"/>
+        <v>224</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ca="1" si="1"/>
+        <v>876</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -924,24 +970,33 @@
       <c r="R5" s="2">
         <v>400</v>
       </c>
-      <c r="S5">
-        <f t="shared" ca="1" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="T5">
-        <f t="shared" ca="1" si="1"/>
-        <v>269</v>
-      </c>
-      <c r="U5">
-        <f t="shared" ca="1" si="1"/>
-        <v>517</v>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
       </c>
       <c r="V5">
         <f t="shared" ca="1" si="1"/>
-        <v>761</v>
+        <v>865</v>
+      </c>
+      <c r="W5">
+        <f t="shared" ca="1" si="1"/>
+        <v>173</v>
+      </c>
+      <c r="X5">
+        <f t="shared" ca="1" si="1"/>
+        <v>624</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" ca="1" si="1"/>
+        <v>957</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -993,24 +1048,33 @@
       <c r="R6" s="2">
         <v>5000</v>
       </c>
-      <c r="S6">
-        <f t="shared" ca="1" si="1"/>
-        <v>852</v>
-      </c>
-      <c r="T6">
-        <f t="shared" ca="1" si="1"/>
-        <v>810</v>
-      </c>
-      <c r="U6">
-        <f t="shared" ca="1" si="1"/>
-        <v>981</v>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
       </c>
       <c r="V6">
         <f t="shared" ca="1" si="1"/>
-        <v>956</v>
+        <v>650</v>
+      </c>
+      <c r="W6">
+        <f t="shared" ca="1" si="1"/>
+        <v>489</v>
+      </c>
+      <c r="X6">
+        <f t="shared" ca="1" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" ca="1" si="1"/>
+        <v>683</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1059,24 +1123,33 @@
       <c r="R7" s="2">
         <v>100</v>
       </c>
-      <c r="S7">
-        <f t="shared" ca="1" si="1"/>
-        <v>933</v>
-      </c>
-      <c r="T7">
-        <f t="shared" ca="1" si="1"/>
-        <v>747</v>
-      </c>
-      <c r="U7">
-        <f t="shared" ca="1" si="1"/>
-        <v>707</v>
+      <c r="S7" s="2">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0</v>
       </c>
       <c r="V7">
         <f t="shared" ca="1" si="1"/>
-        <v>920</v>
+        <v>274</v>
+      </c>
+      <c r="W7">
+        <f t="shared" ca="1" si="1"/>
+        <v>723</v>
+      </c>
+      <c r="X7">
+        <f t="shared" ca="1" si="1"/>
+        <v>938</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" ca="1" si="1"/>
+        <v>919</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1125,24 +1198,33 @@
       <c r="R8" s="2">
         <v>200</v>
       </c>
-      <c r="S8">
-        <f t="shared" ca="1" si="1"/>
-        <v>523</v>
-      </c>
-      <c r="T8">
-        <f t="shared" ca="1" si="1"/>
-        <v>601</v>
-      </c>
-      <c r="U8">
-        <f t="shared" ca="1" si="1"/>
-        <v>708</v>
+      <c r="S8" s="2">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0</v>
       </c>
       <c r="V8">
         <f t="shared" ca="1" si="1"/>
-        <v>733</v>
+        <v>833</v>
+      </c>
+      <c r="W8">
+        <f t="shared" ca="1" si="1"/>
+        <v>754</v>
+      </c>
+      <c r="X8">
+        <f t="shared" ca="1" si="1"/>
+        <v>514</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" ca="1" si="1"/>
+        <v>622</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1194,24 +1276,33 @@
       <c r="R9" s="2">
         <v>700</v>
       </c>
-      <c r="S9">
-        <f t="shared" ca="1" si="1"/>
-        <v>985</v>
-      </c>
-      <c r="T9">
-        <f t="shared" ca="1" si="1"/>
-        <v>853</v>
-      </c>
-      <c r="U9">
-        <f t="shared" ca="1" si="1"/>
-        <v>262</v>
+      <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0</v>
       </c>
       <c r="V9">
         <f t="shared" ca="1" si="1"/>
-        <v>364</v>
+        <v>787</v>
+      </c>
+      <c r="W9">
+        <f t="shared" ca="1" si="1"/>
+        <v>698</v>
+      </c>
+      <c r="X9">
+        <f t="shared" ca="1" si="1"/>
+        <v>773</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" ca="1" si="1"/>
+        <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1263,24 +1354,33 @@
       <c r="R10" s="2">
         <v>450</v>
       </c>
-      <c r="S10">
-        <f t="shared" ca="1" si="1"/>
-        <v>691</v>
-      </c>
-      <c r="T10">
-        <f t="shared" ca="1" si="1"/>
-        <v>361</v>
-      </c>
-      <c r="U10">
-        <f t="shared" ca="1" si="1"/>
-        <v>769</v>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0</v>
       </c>
       <c r="V10">
         <f t="shared" ca="1" si="1"/>
-        <v>672</v>
+        <v>465</v>
+      </c>
+      <c r="W10">
+        <f t="shared" ca="1" si="1"/>
+        <v>533</v>
+      </c>
+      <c r="X10">
+        <f t="shared" ca="1" si="1"/>
+        <v>950</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" ca="1" si="1"/>
+        <v>848</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1332,31 +1432,40 @@
       <c r="R11" s="2">
         <v>1300</v>
       </c>
-      <c r="S11">
-        <f t="shared" ca="1" si="1"/>
-        <v>942</v>
-      </c>
-      <c r="T11">
-        <f t="shared" ca="1" si="1"/>
-        <v>112</v>
-      </c>
-      <c r="U11">
+      <c r="S11" s="2">
+        <v>2000</v>
+      </c>
+      <c r="T11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="U11" s="2">
+        <v>500</v>
+      </c>
+      <c r="V11">
         <f t="shared" ca="1" si="1"/>
         <v>341</v>
       </c>
-      <c r="V11">
-        <f t="shared" ca="1" si="1"/>
-        <v>233</v>
+      <c r="W11">
+        <f t="shared" ca="1" si="1"/>
+        <v>883</v>
+      </c>
+      <c r="X11">
+        <f t="shared" ca="1" si="1"/>
+        <v>283</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" ca="1" si="1"/>
+        <v>959</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid ID" error="Please enter a valid ID" promptTitle="Liberia Project Dashboard ID" prompt="Please do not edit this ID. It is used by the Liberia Project Dashboard to uniquely identify activities." sqref="A2:A11" xr:uid="{30120BDD-722D-034A-B161-CDBDF4B1CEC3}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number" error="Please enter a valid number" sqref="R2:R11" xr:uid="{B6531937-760D-024F-B864-96E601C2FB4D}"/>
     <dataValidation type="date" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid date" error="Please enter a valid date" sqref="E2:F11" xr:uid="{36B9931E-A0F6-A942-9035-C8BA151DA04F}"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Activity Status" error="Your entry is not in the list" promptTitle="Activity Status" prompt="Please select from the list" sqref="D2:D11" xr:uid="{7454DAC1-6059-0B41-9C1E-94721390EFAE}">
       <formula1>"Pipeline/identification,Suspended,Implementation,Ratified,Finalisation,Signed,Closed,Cancelled"</formula1>
     </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number" error="Please enter a valid number" sqref="R2:U11" xr:uid="{B6531937-760D-024F-B864-96E601C2FB4D}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update test data for importing
</commit_message>
<xml_diff>
--- a/tests/artefacts/testdata.xlsx
+++ b/tests/artefacts/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/odi/liberia/aims/tests/artefacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EB354B-5E48-8A48-9D2D-2CCE107E3F0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A898D95B-DAE5-384F-92A1-760A0C68F407}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="820" windowWidth="27640" windowHeight="16020" xr2:uid="{0D2C3C09-8642-F64A-A841-4B349051A884}"/>
   </bookViews>
@@ -273,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -281,6 +281,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75600FF7-6925-5A4F-B4D6-2E51A7284D2B}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,21 +756,17 @@
       <c r="V2" s="2">
         <v>0</v>
       </c>
-      <c r="W2">
-        <f ca="1">RANDBETWEEN(100,999)</f>
-        <v>401</v>
-      </c>
-      <c r="X2">
-        <f t="shared" ref="X2:Z2" ca="1" si="0">RANDBETWEEN(100,999)</f>
-        <v>443</v>
-      </c>
-      <c r="Y2">
-        <f t="shared" ca="1" si="0"/>
-        <v>875</v>
-      </c>
-      <c r="Z2">
-        <f t="shared" ca="1" si="0"/>
-        <v>724</v>
+      <c r="W2" s="5">
+        <v>961</v>
+      </c>
+      <c r="X2" s="5">
+        <v>508</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>939</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>523</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -830,21 +827,17 @@
       <c r="V3" s="2">
         <v>0</v>
       </c>
-      <c r="W3">
-        <f t="shared" ref="W3:Z11" ca="1" si="1">RANDBETWEEN(100,999)</f>
-        <v>641</v>
-      </c>
-      <c r="X3">
-        <f t="shared" ca="1" si="1"/>
-        <v>379</v>
-      </c>
-      <c r="Y3">
-        <f t="shared" ca="1" si="1"/>
-        <v>335</v>
-      </c>
-      <c r="Z3">
-        <f t="shared" ca="1" si="1"/>
-        <v>183</v>
+      <c r="W3" s="5">
+        <v>380</v>
+      </c>
+      <c r="X3" s="5">
+        <v>942</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>697</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>540</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -908,21 +901,17 @@
       <c r="V4" s="2">
         <v>0</v>
       </c>
-      <c r="W4">
-        <f t="shared" ca="1" si="1"/>
-        <v>890</v>
-      </c>
-      <c r="X4">
-        <f t="shared" ca="1" si="1"/>
-        <v>839</v>
-      </c>
-      <c r="Y4">
-        <f t="shared" ca="1" si="1"/>
-        <v>658</v>
-      </c>
-      <c r="Z4">
-        <f t="shared" ca="1" si="1"/>
-        <v>498</v>
+      <c r="W4" s="5">
+        <v>999</v>
+      </c>
+      <c r="X4" s="5">
+        <v>288</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>107</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>587</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -986,21 +975,17 @@
       <c r="V5" s="2">
         <v>0</v>
       </c>
-      <c r="W5">
-        <f t="shared" ca="1" si="1"/>
-        <v>466</v>
-      </c>
-      <c r="X5">
-        <f t="shared" ca="1" si="1"/>
-        <v>476</v>
-      </c>
-      <c r="Y5">
-        <f t="shared" ca="1" si="1"/>
+      <c r="W5" s="5">
+        <v>394</v>
+      </c>
+      <c r="X5" s="5">
         <v>948</v>
       </c>
-      <c r="Z5">
-        <f t="shared" ca="1" si="1"/>
-        <v>426</v>
+      <c r="Y5" s="5">
+        <v>342</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>734</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -1064,21 +1049,17 @@
       <c r="V6" s="2">
         <v>0</v>
       </c>
-      <c r="W6">
-        <f t="shared" ca="1" si="1"/>
-        <v>179</v>
-      </c>
-      <c r="X6">
-        <f t="shared" ca="1" si="1"/>
-        <v>658</v>
-      </c>
-      <c r="Y6">
-        <f t="shared" ca="1" si="1"/>
-        <v>434</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" ca="1" si="1"/>
-        <v>438</v>
+      <c r="W6" s="5">
+        <v>303</v>
+      </c>
+      <c r="X6" s="5">
+        <v>885</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>109</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -1139,21 +1120,17 @@
       <c r="V7" s="2">
         <v>0</v>
       </c>
-      <c r="W7">
-        <f t="shared" ca="1" si="1"/>
-        <v>456</v>
-      </c>
-      <c r="X7">
-        <f t="shared" ca="1" si="1"/>
-        <v>856</v>
-      </c>
-      <c r="Y7">
-        <f t="shared" ca="1" si="1"/>
-        <v>721</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" ca="1" si="1"/>
-        <v>343</v>
+      <c r="W7" s="5">
+        <v>572</v>
+      </c>
+      <c r="X7" s="5">
+        <v>448</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>777</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -1214,21 +1191,17 @@
       <c r="V8" s="2">
         <v>0</v>
       </c>
-      <c r="W8">
-        <f t="shared" ca="1" si="1"/>
-        <v>754</v>
-      </c>
-      <c r="X8">
-        <f t="shared" ca="1" si="1"/>
-        <v>135</v>
-      </c>
-      <c r="Y8">
-        <f t="shared" ca="1" si="1"/>
-        <v>585</v>
-      </c>
-      <c r="Z8">
-        <f t="shared" ca="1" si="1"/>
-        <v>488</v>
+      <c r="W8" s="5">
+        <v>257</v>
+      </c>
+      <c r="X8" s="5">
+        <v>768</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>723</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -1292,21 +1265,17 @@
       <c r="V9" s="2">
         <v>0</v>
       </c>
-      <c r="W9">
-        <f t="shared" ca="1" si="1"/>
-        <v>211</v>
-      </c>
-      <c r="X9">
-        <f t="shared" ca="1" si="1"/>
-        <v>570</v>
-      </c>
-      <c r="Y9">
-        <f t="shared" ca="1" si="1"/>
-        <v>603</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" ca="1" si="1"/>
-        <v>708</v>
+      <c r="W9" s="5">
+        <v>171</v>
+      </c>
+      <c r="X9" s="5">
+        <v>518</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>273</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -1370,21 +1339,17 @@
       <c r="V10" s="2">
         <v>0</v>
       </c>
-      <c r="W10">
-        <f t="shared" ca="1" si="1"/>
-        <v>389</v>
-      </c>
-      <c r="X10">
-        <f t="shared" ca="1" si="1"/>
-        <v>453</v>
-      </c>
-      <c r="Y10">
-        <f t="shared" ca="1" si="1"/>
-        <v>812</v>
-      </c>
-      <c r="Z10">
-        <f t="shared" ca="1" si="1"/>
-        <v>934</v>
+      <c r="W10" s="5">
+        <v>371</v>
+      </c>
+      <c r="X10" s="5">
+        <v>840</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>881</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -1448,21 +1413,17 @@
       <c r="V11" s="2">
         <v>500</v>
       </c>
-      <c r="W11">
-        <f t="shared" ca="1" si="1"/>
-        <v>193</v>
-      </c>
-      <c r="X11">
-        <f t="shared" ca="1" si="1"/>
-        <v>731</v>
-      </c>
-      <c r="Y11">
-        <f t="shared" ca="1" si="1"/>
-        <v>996</v>
-      </c>
-      <c r="Z11">
-        <f t="shared" ca="1" si="1"/>
-        <v>707</v>
+      <c r="W11" s="5">
+        <v>614.35</v>
+      </c>
+      <c r="X11" s="5">
+        <v>103</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>255</v>
+      </c>
+      <c r="Z11" s="5">
+        <v>866.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>